<commit_message>
Upload correzioni primo invio
Corretti i casi di test 3 e 4 per VPS.
ID 26 e 27
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#070104000000XX/ASL4/OASIS4/V.9.9.0/report-checklist.xlsx
+++ b/GATEWAY/A1#070104000000XX/ASL4/OASIS4/V.9.9.0/report-checklist.xlsx
@@ -541,13 +541,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-03-12T14:14:14Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c93723c1ad810d5a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.70.4.4.b8a94729688480590c90a8f1465282237c5d2ed760ac61783627461658867f66.8055c997ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-03-15T14:21:54Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2b9abdabdf5a98f3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.70.4.4.b8a94729688480590c90a8f1465282237c5d2ed760ac61783627461658867f66.f832cde74f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_VPS_CT4</t>
@@ -558,13 +558,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-03-12T14:14:15Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a47dd703ddc31fd4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.70.4.4.b8a94729688480590c90a8f1465282237c5d2ed760ac61783627461658867f66.925ce43f63^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-03-15T14:21:56Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">068b81dc8487bf50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.70.4.4.b8a94729688480590c90a8f1465282237c5d2ed760ac61783627461658867f66.e5515064ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
@@ -5626,11 +5626,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="I134" activeCellId="0" sqref="I134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6520,7 +6520,7 @@
         <v>125</v>
       </c>
       <c r="F24" s="27" t="n">
-        <v>45363</v>
+        <v>45366</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>126</v>
@@ -6564,7 +6564,7 @@
         <v>130</v>
       </c>
       <c r="F25" s="27" t="n">
-        <v>45363</v>
+        <v>45366</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>131</v>

</xml_diff>